<commit_message>
Aggiornamento UCs Utenza + DD
Aggiornato DD inserendo dizionario per l'azienda
Modificati i casi d'uso riguardo la segnalazione (condizioni)
Modificato il caso d'uso della visualizzazione del profilo modificando la condizione
</commit_message>
<xml_diff>
--- a/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
+++ b/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Eat-Reorder\Documents\Eat&amp;Reorder - Use Cases documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916D5CD0-2E6B-4D9D-9935-86D8AF4C9423}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4111F3A2-38F8-473A-AB98-68AED7EB186A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8190" yWindow="2355" windowWidth="21570" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
   <si>
     <t>Attributo</t>
   </si>
@@ -178,6 +178,21 @@
   </si>
   <si>
     <t>Non fate caso alla roba di sotto</t>
+  </si>
+  <si>
+    <t>numero ordine</t>
+  </si>
+  <si>
+    <t>Numero ordine è una stringa di caratteri numerici</t>
+  </si>
+  <si>
+    <t>DD_Seg</t>
+  </si>
+  <si>
+    <t>descrizione problema</t>
+  </si>
+  <si>
+    <t>Descrizione problema è una stringa di caratteri alfanumerici che descrive il problema riscontrato durante un ordine</t>
   </si>
 </sst>
 </file>
@@ -351,15 +366,6 @@
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -373,6 +379,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -653,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,359 +694,401 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="12" t="s">
+      <c r="B18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="12" t="s">
+      <c r="B19" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="14" t="s">
+      <c r="B20" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="4"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="12" t="s">
+      <c r="B30" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="14" t="s">
+      <c r="B31" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="4"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="17"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="9" t="s">
+      <c r="B35" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="16"/>
+      <c r="C37" s="17"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>13</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B50" t="s">
         <v>14</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C50" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>16</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B51" t="s">
         <v>9</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C51" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A37:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modifica flussi UCs + PS + DD
Modificati i flussi di alcuni UCs
Modificato il Problem Statement
Modificato il Dizionario dei Dati
</commit_message>
<xml_diff>
--- a/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
+++ b/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Eat-Reorder\Documents\Eat&amp;Reorder - Use Cases documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4111F3A2-38F8-473A-AB98-68AED7EB186A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5E66D9-2E0C-4355-94CD-667A261D9098}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7230" yWindow="4215" windowWidth="21570" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="71">
   <si>
     <t>Attributo</t>
   </si>
@@ -75,12 +75,6 @@
     <t>Carta di credito è una stringa di 16 caratteri numerici</t>
   </si>
   <si>
-    <t>indirizzo di destinazione</t>
-  </si>
-  <si>
-    <t>Indirizzo del cliente</t>
-  </si>
-  <si>
     <t>via</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>DD_Log</t>
   </si>
   <si>
-    <t>Non fate caso alla roba di sotto</t>
-  </si>
-  <si>
     <t>numero ordine</t>
   </si>
   <si>
@@ -193,6 +184,60 @@
   </si>
   <si>
     <t>Descrizione problema è una stringa di caratteri alfanumerici che descrive il problema riscontrato durante un ordine</t>
+  </si>
+  <si>
+    <t>DD_QtOrd</t>
+  </si>
+  <si>
+    <t>quantità</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La quantità indica il numero di prodotti che si vuole acquistare e deve essere 1 &lt;= quantità &lt;= 50 </t>
+  </si>
+  <si>
+    <t>DD_Ord</t>
+  </si>
+  <si>
+    <t>note ordine</t>
+  </si>
+  <si>
+    <t>Via in cui è necessario consegnare l'ordine</t>
+  </si>
+  <si>
+    <t>Numero civico legato alla via in cui consegnare l'ordine</t>
+  </si>
+  <si>
+    <t>Città di consegna dell'ordine</t>
+  </si>
+  <si>
+    <t>Note ordine è una stringa che descrive eventuali noti riguardanti l'ordine</t>
+  </si>
+  <si>
+    <t>DD_Prd</t>
+  </si>
+  <si>
+    <t>descrizione</t>
+  </si>
+  <si>
+    <t>immagine</t>
+  </si>
+  <si>
+    <t>prezzo</t>
+  </si>
+  <si>
+    <t>Nome del prodotto</t>
+  </si>
+  <si>
+    <t>Descrizione del prodotto</t>
+  </si>
+  <si>
+    <t>Immagine</t>
+  </si>
+  <si>
+    <t>Immagine illustrativa del prodotto</t>
+  </si>
+  <si>
+    <t>Prezzo del prodotto</t>
   </si>
 </sst>
 </file>
@@ -216,7 +261,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -359,11 +404,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -379,6 +463,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -668,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,11 +784,11 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
+      <c r="A3" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="23"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -746,11 +836,11 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
+      <c r="A9" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="23"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -782,95 +872,95 @@
         <v>9</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -879,11 +969,11 @@
       <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
+      <c r="A22" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="22"/>
+      <c r="C22" s="23"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -915,7 +1005,7 @@
         <v>9</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -926,71 +1016,71 @@
         <v>9</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="17"/>
+      <c r="A33" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="22"/>
+      <c r="C33" s="23"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
@@ -1016,32 +1106,32 @@
     </row>
     <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="17"/>
+      <c r="A37" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="22"/>
+      <c r="C37" s="23"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1055,35 +1145,166 @@
         <v>7</v>
       </c>
     </row>
+    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="16"/>
+      <c r="C42" s="17"/>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="22"/>
+      <c r="C45" s="23"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>50</v>
+      <c r="A49" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>14</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>16</v>
-      </c>
-      <c r="B51" t="s">
+    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54" s="22"/>
+      <c r="C54" s="23"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C51" t="s">
-        <v>17</v>
+      <c r="C55" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A45:C45"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A22:C22"/>

</xml_diff>

<commit_message>
Modificato il Report e aggiornato il caso Login
Rimosso controllo dati da Login
Aggiunti UC IDs al Report
</commit_message>
<xml_diff>
--- a/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
+++ b/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Eat-Reorder\Documents\Eat&amp;Reorder - Use Cases documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5E66D9-2E0C-4355-94CD-667A261D9098}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE078D06-7086-4B19-B778-9DA4AEF44952}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7230" yWindow="4215" windowWidth="21570" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="70">
   <si>
     <t>Attributo</t>
   </si>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t>DD_Fat</t>
-  </si>
-  <si>
-    <t>DD_Log</t>
   </si>
   <si>
     <t>numero ordine</t>
@@ -447,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -469,6 +466,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -758,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,11 +790,11 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="26"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -836,11 +842,11 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="26"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -969,11 +975,11 @@
       <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="23"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="26"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -1077,239 +1083,205 @@
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B33" s="22"/>
       <c r="C33" s="23"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="B36" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="23"/>
-    </row>
+    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="1" t="s">
+      <c r="A38" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="16"/>
+      <c r="C38" s="17"/>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="22"/>
+      <c r="C41" s="23"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B42" s="16"/>
-      <c r="C42" s="17"/>
-    </row>
-    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B45" s="22"/>
-      <c r="C45" s="23"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B46" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>58</v>
+      <c r="C46" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>25</v>
-      </c>
+      <c r="A50" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" s="22"/>
+      <c r="C50" s="23"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C51" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B54" s="22"/>
-      <c r="C54" s="23"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C57" s="3" t="s">
+      <c r="C54" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A45:C45"/>
+  <mergeCells count="3">
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A37:C37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactoring Casi d'Uso pre-RAD
Refctorizzati i casi d'uso.
Ad alcuni casi d'uso è stato modificato il flusso di eventi, riadattandoli al report.
A molti casi d'uso è stata modificata tabulazione e sintassi di alcune parole.
Alcuni casi d'uso sono stati riadattati secondo i mockups
Modificato il dizionario dei dati, rimuovendo le ridondanze
Riadattato il problem statement in seguito ad alcune modifiche
Aggiornato il report precisando alcuni dettagli su alcune situazioni
</commit_message>
<xml_diff>
--- a/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
+++ b/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Eat-Reorder\Documents\Eat&amp;Reorder - Use Cases documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE078D06-7086-4B19-B778-9DA4AEF44952}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3303C82C-F3D2-492E-ADEA-AAA21A68ED0F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10710" yWindow="4200" windowWidth="21570" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
   <si>
     <t>Attributo</t>
   </si>
@@ -198,15 +198,6 @@
     <t>note ordine</t>
   </si>
   <si>
-    <t>Via in cui è necessario consegnare l'ordine</t>
-  </si>
-  <si>
-    <t>Numero civico legato alla via in cui consegnare l'ordine</t>
-  </si>
-  <si>
-    <t>Città di consegna dell'ordine</t>
-  </si>
-  <si>
     <t>Note ordine è una stringa che descrive eventuali noti riguardanti l'ordine</t>
   </si>
   <si>
@@ -235,6 +226,12 @@
   </si>
   <si>
     <t>Prezzo del prodotto</t>
+  </si>
+  <si>
+    <t>indirizzo di destinazione</t>
+  </si>
+  <si>
+    <t>Stringa contenente via e numero civico</t>
   </si>
 </sst>
 </file>
@@ -258,7 +255,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -401,50 +398,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -463,9 +421,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -764,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,11 +763,11 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -842,11 +815,11 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="26"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -975,11 +948,11 @@
       <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="29"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -1099,182 +1072,135 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
+    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="9" t="s">
+      <c r="B35" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="17"/>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+      <c r="B37" s="16"/>
+      <c r="C37" s="17"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="25"/>
+      <c r="C40" s="26"/>
+    </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B41" s="22"/>
-      <c r="C41" s="23"/>
+      <c r="A41" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C42" s="20" t="s">
+      <c r="A42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C43" s="9" t="s">
+    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="B45" s="19"/>
+      <c r="C45" s="20"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C47" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B50" s="22"/>
-      <c r="C50" s="23"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52" s="3" t="s">
+      <c r="C49" s="6" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update DD - Dizionario dei Dati.xlsx
aggiornato il dizionario dei dati inserendo la lunghezza di ogni attributo
</commit_message>
<xml_diff>
--- a/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
+++ b/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Eat-Reorder\Documents\Eat&amp;Reorder - Use Cases documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincenzo\Documents\GitHub\Eat-Reorder\Documents\Eat&amp;Reorder - Use Cases documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3303C82C-F3D2-492E-ADEA-AAA21A68ED0F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55033C9-F5D6-4468-A48E-BBA43FFECC6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10710" yWindow="4200" windowWidth="21570" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="90">
   <si>
     <t>Attributo</t>
   </si>
@@ -232,6 +232,69 @@
   </si>
   <si>
     <t>Stringa contenente via e numero civico</t>
+  </si>
+  <si>
+    <t>Lunghezza</t>
+  </si>
+  <si>
+    <t>non deve essere vuota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">almeno 7 caratteri massimo 20 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">almeno 3 caratteri massimo 20 </t>
+  </si>
+  <si>
+    <t>almeno 7 caratteri massimo 20</t>
+  </si>
+  <si>
+    <t>almeno 3 caratteri massimo 20</t>
+  </si>
+  <si>
+    <t>almeno 1 carattere massimo 3</t>
+  </si>
+  <si>
+    <t>almeno 4 caratteri massimo 15</t>
+  </si>
+  <si>
+    <t>9 o 10 numeri</t>
+  </si>
+  <si>
+    <t>11 caratteri</t>
+  </si>
+  <si>
+    <t>da 00:00 a 23:59</t>
+  </si>
+  <si>
+    <t>almeno 4 caratteri massimo 20</t>
+  </si>
+  <si>
+    <t>almeno 1 numero</t>
+  </si>
+  <si>
+    <t>almeno 20 caratteri massimo 250 caratteri</t>
+  </si>
+  <si>
+    <t>deve essere maggiore di 1 e minore di 50</t>
+  </si>
+  <si>
+    <t>16 numeri</t>
+  </si>
+  <si>
+    <t>almeno 10 caratteri massimo 150</t>
+  </si>
+  <si>
+    <t>almeno 1 carattere massimo 25</t>
+  </si>
+  <si>
+    <t>almeno 10 carattere massimo 250</t>
+  </si>
+  <si>
+    <t>deve esserci un immagine</t>
+  </si>
+  <si>
+    <t>numero decimale maggiore uguale a 0</t>
   </si>
 </sst>
 </file>
@@ -255,7 +318,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -398,11 +461,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -457,6 +559,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -737,477 +850,593 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="141.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="36.21875" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="141.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="30"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="30"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="D14" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="D16" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="D17" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="D19" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12"/>
-      <c r="B21" s="7"/>
+      <c r="B21" s="12"/>
       <c r="C21" s="7"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="30"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="29"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="D25" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="D26" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="D27" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="D28" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="D29" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="D30" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="D31" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="23"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="35"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="23"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="D35" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="12"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="17"/>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="36"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="17"/>
+    </row>
+    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="26"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="35"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="26"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="D41" s="9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="D43" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="7"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="19"/>
-      <c r="C45" s="20"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="35"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="20"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="D49" s="6" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A22:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Aggiornato UC Ordinazione, DD e Report
Aggiunta precondizione RF3
Aggiornato DD rimuovendo il controllo degli orari per l'azienda
Aggiornato Report specificando il controllo degli orari per l'azienda
</commit_message>
<xml_diff>
--- a/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
+++ b/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincenzo\Documents\GitHub\Eat-Reorder\Documents\Eat&amp;Reorder - Use Cases documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Eat-Reorder\Documents\Eat&amp;Reorder - Use Cases documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55033C9-F5D6-4468-A48E-BBA43FFECC6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2FD4C5-B2F2-4E93-92BE-0FF7A011973C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="86">
   <si>
     <t>Attributo</t>
   </si>
@@ -90,12 +90,6 @@
     <t>partita iva</t>
   </si>
   <si>
-    <t>orario di apertura</t>
-  </si>
-  <si>
-    <t>orario di chiusura</t>
-  </si>
-  <si>
     <t>Nome dell'azienda</t>
   </si>
   <si>
@@ -106,12 +100,6 @@
   </si>
   <si>
     <t>Partita iva è una stringa di 11 caratteri alfanumerici</t>
-  </si>
-  <si>
-    <t>Orario di apertura indica l'orario in cui l'azienda diventa operativa e deve rispettare il seguente formato: HH:MM, dove HH è l'ora e MM sono i minuti</t>
-  </si>
-  <si>
-    <t>Orario di chiusura indica l'orario in cui l'azienda smette di essere operativa e deve rispettare il seguente formato: HH:MM, dove HH è l'ora e MM sono i minuti</t>
   </si>
   <si>
     <t>Via in cui è locata l'azienda</t>
@@ -318,7 +306,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -500,11 +488,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -532,7 +538,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -541,35 +558,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -850,26 +840,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" customWidth="1"/>
-    <col min="2" max="2" width="36.21875" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="141.88671875" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="141.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -878,21 +868,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="29"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="30"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="31" t="s">
-        <v>70</v>
+      <c r="B4" s="21" t="s">
+        <v>66</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -901,12 +891,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="31" t="s">
-        <v>71</v>
+      <c r="B5" s="21" t="s">
+        <v>67</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -915,12 +905,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="31" t="s">
-        <v>72</v>
+      <c r="B6" s="21" t="s">
+        <v>68</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
@@ -929,12 +919,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="32" t="s">
-        <v>72</v>
+      <c r="B7" s="22" t="s">
+        <v>68</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>9</v>
@@ -943,21 +933,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="29"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="31" t="s">
-        <v>70</v>
+      <c r="B10" s="21" t="s">
+        <v>66</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -966,12 +956,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="31" t="s">
-        <v>73</v>
+      <c r="B11" s="21" t="s">
+        <v>69</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -980,463 +970,434 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="31" t="s">
-        <v>74</v>
+      <c r="B12" s="21" t="s">
+        <v>70</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D13" s="32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>75</v>
+        <v>26</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>71</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="31" t="s">
-        <v>76</v>
+      <c r="B15" s="21" t="s">
+        <v>72</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="31" t="s">
-        <v>76</v>
+      <c r="B16" s="21" t="s">
+        <v>72</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="31" t="s">
-        <v>77</v>
+      <c r="B17" s="21" t="s">
+        <v>73</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="B18" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="8" t="s">
+      <c r="D18" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="25"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="29"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="31" t="s">
+      <c r="D22" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="31" t="s">
+      <c r="C23" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="33" t="s">
-        <v>74</v>
-      </c>
       <c r="C25" s="8" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="33" t="s">
-        <v>74</v>
+        <v>29</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>76</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="33" t="s">
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="25"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="20"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="33" t="s">
+      <c r="D32" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="26"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="17"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="25"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="20"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="25"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="20"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="C30" s="8" t="s">
+      <c r="D44" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="35"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="23"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B34" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="D45" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="17"/>
-    </row>
-    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B40" s="35"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="26"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B45" s="35"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="20"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B46" s="31" t="s">
-        <v>86</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" s="3" t="s">
+      <c r="D47" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B48" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B49" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A22:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Apportate modifiche al Dizionario dei Dati
</commit_message>
<xml_diff>
--- a/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
+++ b/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Eat-Reorder\Documents\Eat&amp;Reorder - Use Cases documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\Eat-Reorder\Documents\Eat&amp;Reorder - Use Cases documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2FD4C5-B2F2-4E93-92BE-0FF7A011973C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5894A597-317E-4981-93F2-A2759C25FD86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="82">
   <si>
     <t>Attributo</t>
   </si>
@@ -195,9 +195,6 @@
     <t>descrizione</t>
   </si>
   <si>
-    <t>immagine</t>
-  </si>
-  <si>
     <t>prezzo</t>
   </si>
   <si>
@@ -207,12 +204,6 @@
     <t>Descrizione del prodotto</t>
   </si>
   <si>
-    <t>Immagine</t>
-  </si>
-  <si>
-    <t>Immagine illustrativa del prodotto</t>
-  </si>
-  <si>
     <t>Prezzo del prodotto</t>
   </si>
   <si>
@@ -261,12 +252,6 @@
     <t>almeno 1 numero</t>
   </si>
   <si>
-    <t>almeno 20 caratteri massimo 250 caratteri</t>
-  </si>
-  <si>
-    <t>deve essere maggiore di 1 e minore di 50</t>
-  </si>
-  <si>
     <t>16 numeri</t>
   </si>
   <si>
@@ -279,10 +264,13 @@
     <t>almeno 10 carattere massimo 250</t>
   </si>
   <si>
-    <t>deve esserci un immagine</t>
-  </si>
-  <si>
     <t>numero decimale maggiore uguale a 0</t>
+  </si>
+  <si>
+    <t>almeno 10 caratteri massimo 250 caratteri</t>
+  </si>
+  <si>
+    <t>maggiore di 0 e minore uguale di 50</t>
   </si>
 </sst>
 </file>
@@ -546,6 +534,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -558,8 +548,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -840,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +847,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -870,19 +858,19 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="32"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -896,7 +884,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -910,7 +898,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
@@ -924,7 +912,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>9</v>
@@ -935,19 +923,19 @@
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -961,7 +949,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -975,7 +963,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>9</v>
@@ -985,16 +973,16 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="28" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1003,7 +991,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>27</v>
@@ -1017,7 +1005,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>9</v>
@@ -1031,7 +1019,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>9</v>
@@ -1045,7 +1033,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>14</v>
@@ -1059,7 +1047,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>4</v>
@@ -1087,7 +1075,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>4</v>
@@ -1101,7 +1089,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>4</v>
@@ -1115,7 +1103,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>9</v>
@@ -1129,7 +1117,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>9</v>
@@ -1143,7 +1131,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>14</v>
@@ -1157,7 +1145,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>9</v>
@@ -1171,7 +1159,7 @@
         <v>30</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>9</v>
@@ -1185,7 +1173,7 @@
         <v>31</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>4</v>
@@ -1199,7 +1187,7 @@
         <v>32</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>4</v>
@@ -1222,7 +1210,7 @@
         <v>43</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>14</v>
@@ -1236,7 +1224,7 @@
         <v>46</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>4</v>
@@ -1264,7 +1252,7 @@
         <v>49</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>27</v>
@@ -1284,16 +1272,16 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1301,7 +1289,7 @@
         <v>13</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>14</v>
@@ -1315,7 +1303,7 @@
         <v>52</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>4</v>
@@ -1343,13 +1331,13 @@
         <v>8</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1357,41 +1345,27 @@
         <v>55</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D45" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="6" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1400,5 +1374,6 @@
     <mergeCell ref="A9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modifica Caso d'uso Ordinazione + modifica campo Indirizzo di destinazione
Apportata modifica al caso d'uso Ordinazione
Aggiunti campi (via, numero civico, città, provincia) all'interno del dizionario dei dati
</commit_message>
<xml_diff>
--- a/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
+++ b/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\Eat-Reorder\Documents\Eat&amp;Reorder - Use Cases documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5894A597-317E-4981-93F2-A2759C25FD86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AF7D44-9DF2-4C39-A0B1-5C8CA5750229}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5235" yWindow="570" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="80">
   <si>
     <t>Attributo</t>
   </si>
@@ -205,12 +205,6 @@
   </si>
   <si>
     <t>Prezzo del prodotto</t>
-  </si>
-  <si>
-    <t>indirizzo di destinazione</t>
-  </si>
-  <si>
-    <t>Stringa contenente via e numero civico</t>
   </si>
   <si>
     <t>Lunghezza</t>
@@ -498,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -548,6 +542,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -828,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,7 +842,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -870,7 +865,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -884,7 +879,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -898,7 +893,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
@@ -912,7 +907,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>9</v>
@@ -935,7 +930,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -949,7 +944,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -963,7 +958,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>9</v>
@@ -977,7 +972,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>9</v>
@@ -991,7 +986,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>27</v>
@@ -1005,7 +1000,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>9</v>
@@ -1019,7 +1014,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>9</v>
@@ -1033,7 +1028,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>14</v>
@@ -1047,7 +1042,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>4</v>
@@ -1075,7 +1070,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>4</v>
@@ -1089,7 +1084,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>4</v>
@@ -1103,7 +1098,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>9</v>
@@ -1117,7 +1112,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>9</v>
@@ -1131,7 +1126,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>14</v>
@@ -1145,7 +1140,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>9</v>
@@ -1159,7 +1154,7 @@
         <v>30</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>9</v>
@@ -1173,7 +1168,7 @@
         <v>31</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>4</v>
@@ -1187,7 +1182,7 @@
         <v>32</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>4</v>
@@ -1210,7 +1205,7 @@
         <v>43</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>14</v>
@@ -1224,7 +1219,7 @@
         <v>46</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>4</v>
@@ -1252,7 +1247,7 @@
         <v>49</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>27</v>
@@ -1271,100 +1266,142 @@
       <c r="D38" s="20"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B39" s="23" t="s">
+      <c r="A39" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" s="21" t="s">
+      <c r="D44" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="25"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="20"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="20"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B44" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B45" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" s="6" t="s">
+      <c r="D49" s="6" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modificato dizionario dei dati per Ordinazione + TC_RFA3-Ordinazione
</commit_message>
<xml_diff>
--- a/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
+++ b/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\Eat-Reorder\Documents\Eat&amp;Reorder - Use Cases documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AF7D44-9DF2-4C39-A0B1-5C8CA5750229}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A8CDCA-85B0-4E88-AC2E-BD21E05FC1EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5235" yWindow="570" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="85">
   <si>
     <t>Attributo</t>
   </si>
@@ -246,12 +246,6 @@
     <t>almeno 1 numero</t>
   </si>
   <si>
-    <t>16 numeri</t>
-  </si>
-  <si>
-    <t>almeno 10 caratteri massimo 150</t>
-  </si>
-  <si>
     <t>almeno 1 carattere massimo 25</t>
   </si>
   <si>
@@ -265,6 +259,27 @@
   </si>
   <si>
     <t>maggiore di 0 e minore uguale di 50</t>
+  </si>
+  <si>
+    <t>via e numero civico</t>
+  </si>
+  <si>
+    <t>Città in cui è locato il cliente che effettua l'ordine</t>
+  </si>
+  <si>
+    <t>Via e numero civico in cui è locato il cliente che effettua l'ordine</t>
+  </si>
+  <si>
+    <t>esattamente 2 caratteri</t>
+  </si>
+  <si>
+    <t>da 0 a massimo 150 caratteri</t>
+  </si>
+  <si>
+    <t>esattamente 16 caratteri numerici</t>
+  </si>
+  <si>
+    <t>almeno 2 caratteri massimo 23 totali</t>
   </si>
 </sst>
 </file>
@@ -492,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -542,7 +557,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -823,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,7 +1233,7 @@
         <v>46</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>4</v>
@@ -1247,7 +1261,7 @@
         <v>49</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>27</v>
@@ -1266,142 +1280,128 @@
       <c r="D38" s="20"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="7" t="s">
+      <c r="A39" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="28" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="D40" s="9" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="25"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="20"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D42" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="25"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="20"/>
+      <c r="D46" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="B47" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B48" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B49" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="C49" s="5" t="s">
+      <c r="C48" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D48" s="6" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Creato TC_Specification per alcuni TC + apportate modifiche al dizionario dei dati
Creato TC_Specification per i seguenti TC:
TC_RFU1.1-RegistrazioneCliente
TC_RFU1.2-RegistrazioneAzienda
TC_RFU2-Login
Sono state apportate alcune modifiche al dizionario dei dati, legate al formato della provincia.
</commit_message>
<xml_diff>
--- a/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
+++ b/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\Eat-Reorder\Documents\Eat&amp;Reorder - Use Cases documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A8CDCA-85B0-4E88-AC2E-BD21E05FC1EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5530A34-D5BF-4369-BEF8-BE7D5A0246FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3855" yWindow="1020" windowWidth="15375" windowHeight="9225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="84">
   <si>
     <t>Attributo</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Città in cui consegna il fattorino</t>
   </si>
   <si>
-    <t>Provincia della città, composta ad due caratteri</t>
-  </si>
-  <si>
     <t>Provincia della città, composta da due caratteri</t>
   </si>
   <si>
@@ -234,9 +231,6 @@
     <t>9 o 10 numeri</t>
   </si>
   <si>
-    <t>11 caratteri</t>
-  </si>
-  <si>
     <t>da 00:00 a 23:59</t>
   </si>
   <si>
@@ -280,6 +274,9 @@
   </si>
   <si>
     <t>almeno 2 caratteri massimo 23 totali</t>
+  </si>
+  <si>
+    <t>esattamente 11 caratteri</t>
   </si>
 </sst>
 </file>
@@ -839,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +853,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -868,7 +865,7 @@
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="31"/>
@@ -879,7 +876,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -893,7 +890,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -907,7 +904,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
@@ -921,7 +918,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>9</v>
@@ -933,7 +930,7 @@
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -944,7 +941,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -958,7 +955,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -972,10 +969,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>21</v>
@@ -986,7 +983,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>9</v>
@@ -1000,7 +997,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>27</v>
@@ -1014,7 +1011,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>9</v>
@@ -1028,7 +1025,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>9</v>
@@ -1042,7 +1039,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>14</v>
@@ -1056,10 +1053,10 @@
         <v>20</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>24</v>
@@ -1073,7 +1070,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="25"/>
       <c r="C20" s="19"/>
@@ -1084,7 +1081,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>4</v>
@@ -1098,7 +1095,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>4</v>
@@ -1112,7 +1109,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>9</v>
@@ -1126,7 +1123,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>9</v>
@@ -1140,7 +1137,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>14</v>
@@ -1154,7 +1151,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>9</v>
@@ -1168,13 +1165,13 @@
         <v>30</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1182,13 +1179,13 @@
         <v>31</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1196,19 +1193,19 @@
         <v>32</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="25"/>
       <c r="C31" s="19"/>
@@ -1216,30 +1213,30 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1250,7 +1247,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" s="26"/>
       <c r="C35" s="16"/>
@@ -1258,22 +1255,22 @@
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B38" s="25"/>
       <c r="C38" s="19"/>
@@ -1281,16 +1278,16 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1298,13 +1295,13 @@
         <v>17</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1312,13 +1309,13 @@
         <v>18</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1326,7 +1323,7 @@
         <v>13</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>14</v>
@@ -1337,16 +1334,16 @@
     </row>
     <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1357,7 +1354,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B45" s="25"/>
       <c r="C45" s="19"/>
@@ -1368,41 +1365,41 @@
         <v>8</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rivisionati alcuni CategoryPartition e approvati alcuni TC
Sono stati rivisionati alcuni CategoryPartition ed apportate alcune modifiche ai TC:
TC_RFU3.2-ModificaProfiloAzienda
TC_RFU3.2-ModificaProfiloFattorino

Bisogna rifare i TC_Specification per le combinazioni che includono nuovi CategoryPartition.
E' stato ulteriormente modificato il Dizionario dei Dati

Sono stati controllati ed approvati i seguenti TC:
TC_RFU4-CreaSegnalazioneAzienda
TC_RFU5-GestisciSegnalazioneAzienda
</commit_message>
<xml_diff>
--- a/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
+++ b/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\Eat-Reorder\Documents\Eat&amp;Reorder - Use Cases documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5530A34-D5BF-4369-BEF8-BE7D5A0246FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7684CFE-AB34-4FE8-9D80-3242BA169D00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3855" yWindow="1020" windowWidth="15375" windowHeight="9225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -836,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,7 +1165,7 @@
         <v>30</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Creato TC_Specification per TC_RFA3-Ordinazione
E' stato creato il TC_Specification per TC_RFA3-Ordinazione
Apportate modifiche ai seguenti TC legati ad errori sintattici e incongruenze con i nomi dei TEST_CASE_ID:
TC_RFU1.2-RegistrazioneAzienda
TC_RFU1.3-RegistrazioneFattorino
Apportate modifiche al Dizionario per l'attributo DD_FAT:
Cancellato Orario inizio consegna/Orario fine consegna

Co-Authored-By: Vincenzo De Martino <kenz097@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
+++ b/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\Eat-Reorder\Documents\Eat&amp;Reorder - Use Cases documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7684CFE-AB34-4FE8-9D80-3242BA169D00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1DB24C-780C-4105-954D-E3773417AE71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3855" yWindow="1020" windowWidth="15375" windowHeight="9225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="79">
   <si>
     <t>Attributo</t>
   </si>
@@ -120,12 +120,6 @@
     <t>provincia di consegna</t>
   </si>
   <si>
-    <t>orario di inizio disponibilità</t>
-  </si>
-  <si>
-    <t>orario di fine disponibilità</t>
-  </si>
-  <si>
     <t>Nome del fattorino</t>
   </si>
   <si>
@@ -138,12 +132,6 @@
     <t>Provincia della città, composta da due caratteri</t>
   </si>
   <si>
-    <t>Orario di inizio disponibilità indica l'orario in cui il fattorino diventa operativo e deve rispettare il seguente formato: HH:MM, dove HH è l'ora e MM sono i minuti</t>
-  </si>
-  <si>
-    <t>Orario di fine disponibilità indica l'orario in cui il fattorino smette di essere operativo e deve rispettare il seguente formato: HH:MM, dove HH è l'ora e MM sono i minuti</t>
-  </si>
-  <si>
     <t>DD_Azi</t>
   </si>
   <si>
@@ -231,9 +219,6 @@
     <t>9 o 10 numeri</t>
   </si>
   <si>
-    <t>da 00:00 a 23:59</t>
-  </si>
-  <si>
     <t>almeno 4 caratteri massimo 20</t>
   </si>
   <si>
@@ -273,10 +258,10 @@
     <t>esattamente 16 caratteri numerici</t>
   </si>
   <si>
-    <t>almeno 2 caratteri massimo 23 totali</t>
-  </si>
-  <si>
     <t>esattamente 11 caratteri</t>
+  </si>
+  <si>
+    <t>almeno 1 caratteri massimo 20 totali</t>
   </si>
 </sst>
 </file>
@@ -834,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,7 +838,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -865,7 +850,7 @@
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="31"/>
@@ -876,7 +861,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
@@ -890,7 +875,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -904,7 +889,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
@@ -918,7 +903,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>9</v>
@@ -930,7 +915,7 @@
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -941,7 +926,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -955,7 +940,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -969,7 +954,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>4</v>
@@ -983,7 +968,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>9</v>
@@ -997,7 +982,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>27</v>
@@ -1011,7 +996,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>9</v>
@@ -1025,13 +1010,13 @@
         <v>18</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1039,7 +1024,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>14</v>
@@ -1053,7 +1038,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>27</v>
@@ -1070,7 +1055,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B20" s="25"/>
       <c r="C20" s="19"/>
@@ -1081,7 +1066,7 @@
         <v>3</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>4</v>
@@ -1095,7 +1080,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>4</v>
@@ -1109,13 +1094,13 @@
         <v>8</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1123,13 +1108,13 @@
         <v>11</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1137,7 +1122,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>14</v>
@@ -1151,13 +1136,13 @@
         <v>29</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1165,241 +1150,213 @@
         <v>30</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="25"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="20"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" s="10" t="s">
+      <c r="D31" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="26"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="17"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="25"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="20"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="20"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="26"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="17"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="D37" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="20"/>
+      <c r="A38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B40" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="25"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="20"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C44" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="D44" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B45" s="25"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="20"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B46" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="D46" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="B47" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B48" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test case e dizionario dei dati
TC RFA2.1-RFR1-RFR2-RFU1.1-RFU1.2-RFU1.3 CORRETTI
Dizionario dei dati cambiato (in caso da rivedere)
</commit_message>
<xml_diff>
--- a/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
+++ b/Documents/Eat&Reorder - Use Cases documents/DD - Dizionario dei Dati.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\Eat-Reorder\Documents\Eat&amp;Reorder - Use Cases documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincenzo\Documents\GitHub\Eat-Reorder\Documents\Eat&amp;Reorder - Use Cases documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1DB24C-780C-4105-954D-E3773417AE71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB61FB25-D217-49D8-8576-4CF914A96A04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="1020" windowWidth="15375" windowHeight="9225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="78">
   <si>
     <t>Attributo</t>
   </si>
@@ -213,9 +213,6 @@
     <t>almeno 1 carattere massimo 3</t>
   </si>
   <si>
-    <t>almeno 4 caratteri massimo 15</t>
-  </si>
-  <si>
     <t>9 o 10 numeri</t>
   </si>
   <si>
@@ -243,9 +240,6 @@
     <t>via e numero civico</t>
   </si>
   <si>
-    <t>Città in cui è locato il cliente che effettua l'ordine</t>
-  </si>
-  <si>
     <t>Via e numero civico in cui è locato il cliente che effettua l'ordine</t>
   </si>
   <si>
@@ -261,7 +255,10 @@
     <t>esattamente 11 caratteri</t>
   </si>
   <si>
-    <t>almeno 1 caratteri massimo 20 totali</t>
+    <t>almeno 1 caratteri massimo 30 totali</t>
+  </si>
+  <si>
+    <t>almeno 3 caratteri massimo 27</t>
   </si>
 </sst>
 </file>
@@ -819,21 +816,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="141.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="141.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -847,8 +844,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="29" t="s">
         <v>36</v>
       </c>
@@ -856,7 +853,7 @@
       <c r="C3" s="31"/>
       <c r="D3" s="32"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -870,7 +867,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -884,7 +881,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -898,7 +895,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -912,8 +909,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>35</v>
       </c>
@@ -921,7 +918,7 @@
       <c r="C9" s="31"/>
       <c r="D9" s="32"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -935,7 +932,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -949,7 +946,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -963,12 +960,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>9</v>
@@ -977,7 +974,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -991,12 +988,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>9</v>
@@ -1005,12 +1002,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>9</v>
@@ -1019,12 +1016,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>14</v>
@@ -1033,12 +1030,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>27</v>
@@ -1047,13 +1044,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
         <v>37</v>
       </c>
@@ -1061,7 +1058,7 @@
       <c r="C20" s="19"/>
       <c r="D20" s="20"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
@@ -1075,7 +1072,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>5</v>
       </c>
@@ -1089,7 +1086,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
         <v>8</v>
       </c>
@@ -1103,7 +1100,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
         <v>11</v>
       </c>
@@ -1117,12 +1114,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>14</v>
@@ -1131,12 +1128,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>9</v>
@@ -1145,12 +1142,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>9</v>
@@ -1159,8 +1156,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
         <v>40</v>
       </c>
@@ -1168,12 +1165,12 @@
       <c r="C29" s="19"/>
       <c r="D29" s="20"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>14</v>
@@ -1182,12 +1179,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
         <v>41</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>4</v>
@@ -1196,13 +1193,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
         <v>43</v>
       </c>
@@ -1210,12 +1207,12 @@
       <c r="C33" s="16"/>
       <c r="D33" s="17"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>27</v>
@@ -1224,8 +1221,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
         <v>46</v>
       </c>
@@ -1233,129 +1230,101 @@
       <c r="C36" s="19"/>
       <c r="D36" s="20"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D37" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="22" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C38" s="8" t="s">
+      <c r="C39" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="25"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="20"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="D42" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="20"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B44" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" s="6" t="s">
+      <c r="D44" s="6" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>